<commit_message>
big haul finalizing a priori species
</commit_message>
<xml_diff>
--- a/Data/MainlandAnole_MorphoData.xlsx
+++ b/Data/MainlandAnole_MorphoData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/My Documents/Projects/Mainland Anole Ecomorphs/Code/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46712BAC-11B9-8040-886A-AB0BE6F28C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615AD83D-A2C9-5743-B997-D46CF487D499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7040" yWindow="1700" windowWidth="28800" windowHeight="18000" xr2:uid="{1B72BD69-9FE4-194F-B481-2CD900495CE4}"/>
   </bookViews>
@@ -1568,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D2D142-8432-E24B-B82B-3B8BD36B4AB3}">
   <dimension ref="A1:AG622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175"/>
+    <sheetView tabSelected="1" topLeftCell="A216" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C219" sqref="C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changed the predict and compile functions to be more versatile with outputs
</commit_message>
<xml_diff>
--- a/Data/MainlandAnole_MorphoData.xlsx
+++ b/Data/MainlandAnole_MorphoData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/My Documents/Projects/Mainland Anole Ecomorphs/Code/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615AD83D-A2C9-5743-B997-D46CF487D499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0334C9-F72B-D04F-A825-FCD601D2265C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7040" yWindow="1700" windowWidth="28800" windowHeight="18000" xr2:uid="{1B72BD69-9FE4-194F-B481-2CD900495CE4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2646" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="375">
   <si>
     <t>Collection</t>
   </si>
@@ -1568,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D2D142-8432-E24B-B82B-3B8BD36B4AB3}">
   <dimension ref="A1:AG622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C219" sqref="C219"/>
+    <sheetView tabSelected="1" topLeftCell="A594" zoomScale="141" workbookViewId="0">
+      <selection activeCell="A613" sqref="A612:XFD613"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57704,9 +57704,7 @@
       <c r="D611" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="E611" s="6" t="s">
-        <v>370</v>
-      </c>
+      <c r="E611" s="6"/>
       <c r="F611" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>